<commit_message>
update delete-temp-files script to remove residual jansi and winstone files
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/execution-summary/artifact/script/delete-temp-files.xlsx
+++ b/execution-summary/artifact/script/delete-temp-files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/execution-dashboard-collector/execution-summary/artifact/script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/execution-dashboard/execution-summary/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870C7695-60BC-C44C-B827-5BEA466298E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D514798F-3CE0-414D-B1BF-1A4B885E6490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="16240" windowWidth="51200" windowHeight="15760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="570">
   <si>
     <t>description</t>
   </si>
@@ -1770,6 +1770,15 @@
   </si>
   <si>
     <t>LOOP END</t>
+  </si>
+  <si>
+    <t>jansi-64*.*</t>
+  </si>
+  <si>
+    <t>Delete temp files</t>
+  </si>
+  <si>
+    <t>winstone*.jar</t>
   </si>
 </sst>
 </file>
@@ -2033,6 +2042,10 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2060,10 +2073,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4392,15 +4401,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.5" style="28" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="50" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.6640625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.83203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="49.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="20.5" style="10" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="20.5" style="23" customWidth="1" collapsed="1"/>
@@ -4413,12 +4422,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="24" t="s">
         <v>11</v>
       </c>
@@ -4436,20 +4445,20 @@
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="35"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>561</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="25"/>
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
@@ -4459,10 +4468,10 @@
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="1:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -4584,7 +4593,7 @@
     </row>
     <row r="7" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="29" t="s">
         <v>565</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -4611,7 +4620,7 @@
     </row>
     <row r="8" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
-      <c r="B8" s="37"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="13" t="s">
         <v>13</v>
       </c>
@@ -4636,7 +4645,7 @@
     </row>
     <row r="9" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
-      <c r="B9" s="37"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="13" t="s">
         <v>14</v>
       </c>
@@ -4661,7 +4670,7 @@
     </row>
     <row r="10" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="29" t="s">
         <v>566</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -4739,12 +4748,22 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
+      <c r="A13" s="27" t="s">
+        <v>568</v>
+      </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="C13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>567</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -4758,10 +4777,18 @@
     <row r="14" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="C14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>569</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>

</xml_diff>

<commit_message>
update delete-temp-files with correct regex
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/execution-summary/artifact/script/delete-temp-files.xlsx
+++ b/execution-summary/artifact/script/delete-temp-files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/execution-dashboard/execution-summary/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D514798F-3CE0-414D-B1BF-1A4B885E6490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF45E8-7334-F94C-8A9A-15160F6B9AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1772,13 +1772,13 @@
     <t>LOOP END</t>
   </si>
   <si>
-    <t>jansi-64*.*</t>
-  </si>
-  <si>
     <t>Delete temp files</t>
   </si>
   <si>
-    <t>winstone*.jar</t>
+    <t>jansi-64.+</t>
+  </si>
+  <si>
+    <t>winstone.+\.jar</t>
   </si>
 </sst>
 </file>
@@ -4401,18 +4401,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.5" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.5" style="28" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="50" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.6640625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="37" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="49.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="20.5" style="10" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.5" style="23" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="20.1640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.1640625" style="23" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="1.6640625" style="11" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" style="16" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="12.5" style="17" customWidth="1" collapsed="1"/>
@@ -4749,7 +4749,7 @@
     </row>
     <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="13" t="s">
@@ -4762,7 +4762,7 @@
         <v>548</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>

</xml_diff>

<commit_message>
undo the additional delete files activity
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/execution-summary/artifact/script/delete-temp-files.xlsx
+++ b/execution-summary/artifact/script/delete-temp-files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/execution-dashboard/execution-summary/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBF45E8-7334-F94C-8A9A-15160F6B9AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E604C7C6-3208-0F48-AEFF-D232E9BC45D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="567">
   <si>
     <t>description</t>
   </si>
@@ -1770,15 +1770,6 @@
   </si>
   <si>
     <t>LOOP END</t>
-  </si>
-  <si>
-    <t>Delete temp files</t>
-  </si>
-  <si>
-    <t>jansi-64.+</t>
-  </si>
-  <si>
-    <t>winstone.+\.jar</t>
   </si>
 </sst>
 </file>
@@ -4397,11 +4388,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O300"/>
+  <dimension ref="A1:O298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4748,22 +4739,12 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
-        <v>567</v>
-      </c>
+      <c r="A13" s="27"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>481</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>568</v>
-      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -4777,18 +4758,10 @@
     <row r="14" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>481</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>569</v>
-      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -4988,7 +4961,7 @@
     </row>
     <row r="26" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="13"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -5022,7 +4995,7 @@
     </row>
     <row r="28" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
-      <c r="B28" s="8"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="13"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -9627,40 +9600,6 @@
       <c r="N298" s="15"/>
       <c r="O298" s="3"/>
     </row>
-    <row r="299" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="27"/>
-      <c r="B299" s="5"/>
-      <c r="C299" s="13"/>
-      <c r="D299" s="7"/>
-      <c r="E299" s="7"/>
-      <c r="F299" s="7"/>
-      <c r="G299" s="7"/>
-      <c r="H299" s="7"/>
-      <c r="I299" s="7"/>
-      <c r="J299" s="22"/>
-      <c r="K299" s="3"/>
-      <c r="L299" s="15"/>
-      <c r="M299" s="12"/>
-      <c r="N299" s="15"/>
-      <c r="O299" s="3"/>
-    </row>
-    <row r="300" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A300" s="27"/>
-      <c r="B300" s="5"/>
-      <c r="C300" s="13"/>
-      <c r="D300" s="7"/>
-      <c r="E300" s="7"/>
-      <c r="F300" s="7"/>
-      <c r="G300" s="7"/>
-      <c r="H300" s="7"/>
-      <c r="I300" s="7"/>
-      <c r="J300" s="22"/>
-      <c r="K300" s="3"/>
-      <c r="L300" s="15"/>
-      <c r="M300" s="12"/>
-      <c r="N300" s="15"/>
-      <c r="O300" s="3"/>
-    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -9669,7 +9608,7 @@
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N1 N3:N100 N301:N1048576">
+  <conditionalFormatting sqref="N1 N299:N1048576 N3:N98">
     <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -9680,22 +9619,22 @@
       <formula>LEFT(N1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N101:N300">
+  <conditionalFormatting sqref="N99:N298">
     <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="WARN">
-      <formula>LEFT(N101,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N99,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="FAIL">
-      <formula>LEFT(N101,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N99,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="3" stopIfTrue="1" operator="beginsWith" text="PASS">
-      <formula>LEFT(N101,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N99,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C300" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C298" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D300" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D298" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added logic to delete from old output folders
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/execution-summary/artifact/script/delete-temp-files.xlsx
+++ b/execution-summary/artifact/script/delete-temp-files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/execution-dashboard/execution-summary/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E604C7C6-3208-0F48-AEFF-D232E9BC45D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D34629-E56E-D24E-BC4B-A84418177403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="579">
   <si>
     <t>description</t>
   </si>
@@ -1770,6 +1770,42 @@
   </si>
   <si>
     <t>LOOP END</t>
+  </si>
+  <si>
+    <t>Delete Old Output</t>
+  </si>
+  <si>
+    <t>oldOutput</t>
+  </si>
+  <si>
+    <t>$(syspath|out|base)</t>
+  </si>
+  <si>
+    <t>determine cut off date</t>
+  </si>
+  <si>
+    <t>cutoffDate</t>
+  </si>
+  <si>
+    <t>$(date|addDay|$(sysdate|now|MM/dd/yyyy HH:mm:ss)|-3)</t>
+  </si>
+  <si>
+    <t>lastMod &lt; $(date|stdFormat|${cutoffDate}|epoch)</t>
+  </si>
+  <si>
+    <t>SkipIf( ${foldersNotDeleted} is empty )</t>
+  </si>
+  <si>
+    <t>LOOP START: Delete folders from oldOutput</t>
+  </si>
+  <si>
+    <t>$(array|length|${oldOutput})</t>
+  </si>
+  <si>
+    <t>$(array|item|${oldOutput}|${counter})</t>
+  </si>
+  <si>
+    <t>List folders which are not deleted (but should be)</t>
   </si>
 </sst>
 </file>
@@ -4392,7 +4428,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4403,7 +4439,7 @@
     <col min="4" max="4" width="37" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="49.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="9" width="20.1640625" style="10" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.1640625" style="23" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="41" style="23" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="1.6640625" style="11" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" style="16" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="12.5" style="17" customWidth="1" collapsed="1"/>
@@ -4715,7 +4751,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="5"/>
       <c r="C12" s="13" t="s">
@@ -4731,7 +4767,9 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="22" t="s">
+        <v>574</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="15"/>
       <c r="M12" s="12"/>
@@ -4739,12 +4777,24 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="27" t="s">
+        <v>567</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>572</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -4758,11 +4808,21 @@
     <row r="14" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="C14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>573</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="22"/>
@@ -4775,10 +4835,18 @@
     <row r="15" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="C15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>551</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -4791,11 +4859,21 @@
     </row>
     <row r="16" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="B16" s="29" t="s">
+        <v>575</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>553</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -4808,11 +4886,19 @@
     </row>
     <row r="17" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>555</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -4825,11 +4911,19 @@
     </row>
     <row r="18" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>557</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -4842,11 +4936,21 @@
     </row>
     <row r="19" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="29" t="s">
+        <v>566</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>558</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -4859,12 +4963,24 @@
     </row>
     <row r="20" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="B20" s="5" t="s">
+        <v>578</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>573</v>
+      </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="22"/>
@@ -4874,17 +4990,25 @@
       <c r="N20" s="15"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="C21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>563</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="22"/>
+      <c r="J21" s="22" t="s">
+        <v>574</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="15"/>
       <c r="M21" s="12"/>

</xml_diff>

<commit_message>
update to new saveMatches() command
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/execution-summary/artifact/script/delete-temp-files.xlsx
+++ b/execution-summary/artifact/script/delete-temp-files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/execution-dashboard/execution-summary/artifact/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D34629-E56E-D24E-BC4B-A84418177403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F41D60C-A3A6-3644-928C-556A8A79EB74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="17760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="57600" windowHeight="35540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -27,9 +27,9 @@
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
     <definedName name="excel">'#system'!$I$2:$I$14</definedName>
-    <definedName name="external">'#system'!$J$2:$J$5</definedName>
+    <definedName name="external">'#system'!$J$2:$J$6</definedName>
     <definedName name="image">'#system'!$K$2:$K$7</definedName>
-    <definedName name="io">'#system'!$L$2:$L$29</definedName>
+    <definedName name="io">'#system'!$L$2:$L$30</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$12</definedName>
@@ -48,7 +48,7 @@
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$135</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$138</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="585">
   <si>
     <t>description</t>
   </si>
@@ -823,9 +823,6 @@
     <t>saveAsText(pdf,destination)</t>
   </si>
   <si>
-    <t>assertNotContains(text,substring)</t>
-  </si>
-  <si>
     <t>macro(file,sheet,name)</t>
   </si>
   <si>
@@ -1117,12 +1114,6 @@
     <t>assertLocatorNotPresent(locator)</t>
   </si>
   <si>
-    <t>assertAttributeContains(locator,attrName,contains)</t>
-  </si>
-  <si>
-    <t>assertAttributeNotContains(locator,attrName,contains)</t>
-  </si>
-  <si>
     <t>getRowCount(var)</t>
   </si>
   <si>
@@ -1195,9 +1186,6 @@
     <t>moveTo(var,profile,local,remote)</t>
   </si>
   <si>
-    <t>saveMatches(var,path,filePattern)</t>
-  </si>
-  <si>
     <t>scpCopyFrom(var,profile,remote,local)</t>
   </si>
   <si>
@@ -1634,9 +1622,6 @@
   </si>
   <si>
     <t>tail(id,file)</t>
-  </si>
-  <si>
-    <t>assertTextNotContains(locator,text)</t>
   </si>
   <si>
     <t>typeKeys(os,keystrokes)</t>
@@ -1806,6 +1791,39 @@
   </si>
   <si>
     <t>List folders which are not deleted (but should be)</t>
+  </si>
+  <si>
+    <t>assertNotContain(text,substring)</t>
+  </si>
+  <si>
+    <t>terminate(programName)</t>
+  </si>
+  <si>
+    <t>assertPath(path)</t>
+  </si>
+  <si>
+    <t>saveMatches(var,path,fileFilter,textFilter)</t>
+  </si>
+  <si>
+    <t>assertAttributeContain(locator,attrName,contains)</t>
+  </si>
+  <si>
+    <t>assertAttributeNotContain(locator,attrName,contains)</t>
+  </si>
+  <si>
+    <t>assertTextNotContain(locator,text)</t>
+  </si>
+  <si>
+    <t>saveBrowserVersion(var)</t>
+  </si>
+  <si>
+    <t>saveSelectedText(var,locator)</t>
+  </si>
+  <si>
+    <t>saveSelectedValue(var,locator)</t>
+  </si>
+  <si>
+    <t>(empty)</t>
   </si>
 </sst>
 </file>
@@ -2453,7 +2471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE135"/>
+  <dimension ref="A1:AE138"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
@@ -2469,16 +2487,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="E1" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -2496,22 +2514,22 @@
         <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N1" t="s">
         <v>24</v>
       </c>
       <c r="O1" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="P1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="Q1" t="s">
         <v>192</v>
@@ -2526,19 +2544,19 @@
         <v>51</v>
       </c>
       <c r="U1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="V1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="W1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="X1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="Y1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="Z1" t="s">
         <v>52</v>
@@ -2553,7 +2571,7 @@
         <v>55</v>
       </c>
       <c r="AD1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AE1" t="s">
         <v>223</v>
@@ -2561,19 +2579,19 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="F2" t="s">
         <v>56</v>
@@ -2585,34 +2603,34 @@
         <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="J2" t="s">
         <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="L2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="N2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="O2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="P2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="Q2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="R2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="S2" t="s">
         <v>249</v>
@@ -2621,19 +2639,19 @@
         <v>213</v>
       </c>
       <c r="U2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="V2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="W2" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="X2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="Y2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="Z2" t="s">
         <v>94</v>
@@ -2648,30 +2666,30 @@
         <v>179</v>
       </c>
       <c r="AD2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="AE2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C3" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F3" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H3" t="s">
         <v>86</v>
@@ -2680,28 +2698,28 @@
         <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="K3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="N3" t="s">
         <v>84</v>
       </c>
       <c r="O3" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="P3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="R3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="S3" t="s">
         <v>236</v>
@@ -2710,16 +2728,16 @@
         <v>214</v>
       </c>
       <c r="U3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="W3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="X3" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="Y3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="Z3" t="s">
         <v>95</v>
@@ -2731,7 +2749,7 @@
         <v>173</v>
       </c>
       <c r="AC3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AD3" t="s">
         <v>180</v>
@@ -2742,13 +2760,13 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D4" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -2757,31 +2775,31 @@
         <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="I4" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="J4" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="K4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L4" t="s">
-        <v>234</v>
+        <v>576</v>
       </c>
       <c r="M4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N4" t="s">
         <v>25</v>
       </c>
       <c r="O4" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="P4" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="R4" t="s">
         <v>26</v>
@@ -2793,19 +2811,19 @@
         <v>215</v>
       </c>
       <c r="U4" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="W4" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="X4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="Y4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="Z4" t="s">
-        <v>349</v>
+        <v>578</v>
       </c>
       <c r="AA4" t="s">
         <v>169</v>
@@ -2817,7 +2835,7 @@
         <v>180</v>
       </c>
       <c r="AD4" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="AE4" t="s">
         <v>225</v>
@@ -2825,40 +2843,40 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="B5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="F5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G5" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H5" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="I5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J5" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="K5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L5" t="s">
-        <v>457</v>
+        <v>234</v>
       </c>
       <c r="N5" t="s">
         <v>85</v>
       </c>
       <c r="O5" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="R5" t="s">
         <v>29</v>
@@ -2870,16 +2888,16 @@
         <v>216</v>
       </c>
       <c r="U5" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="W5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="X5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="Z5" t="s">
-        <v>350</v>
+        <v>579</v>
       </c>
       <c r="AA5" t="s">
         <v>170</v>
@@ -2891,7 +2909,7 @@
         <v>181</v>
       </c>
       <c r="AD5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AE5" t="s">
         <v>226</v>
@@ -2902,34 +2920,37 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F6" t="s">
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="H6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I6" t="s">
-        <v>443</v>
+        <v>439</v>
+      </c>
+      <c r="J6" t="s">
+        <v>575</v>
       </c>
       <c r="K6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L6" t="s">
-        <v>70</v>
+        <v>453</v>
       </c>
       <c r="N6" t="s">
         <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="R6" t="s">
         <v>30</v>
@@ -2938,19 +2959,19 @@
         <v>239</v>
       </c>
       <c r="T6" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="U6" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="X6" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="Z6" t="s">
         <v>96</v>
       </c>
       <c r="AA6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="AB6" t="s">
         <v>176</v>
@@ -2959,7 +2980,7 @@
         <v>182</v>
       </c>
       <c r="AD6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AE6" t="s">
         <v>227</v>
@@ -2970,28 +2991,28 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F7" t="s">
         <v>220</v>
       </c>
       <c r="H7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="I7" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="K7" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="N7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="O7" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="R7" t="s">
         <v>32</v>
@@ -3000,19 +3021,19 @@
         <v>240</v>
       </c>
       <c r="T7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="U7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="X7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="Z7" t="s">
         <v>97</v>
       </c>
       <c r="AA7" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="AB7" t="s">
         <v>177</v>
@@ -3021,10 +3042,10 @@
         <v>183</v>
       </c>
       <c r="AD7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="AE7" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
@@ -3032,25 +3053,25 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H8" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L8" t="s">
-        <v>480</v>
+        <v>16</v>
       </c>
       <c r="N8" t="s">
         <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="R8" t="s">
         <v>89</v>
@@ -3059,10 +3080,10 @@
         <v>241</v>
       </c>
       <c r="U8" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="X8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="Z8" t="s">
         <v>98</v>
@@ -3077,10 +3098,10 @@
         <v>184</v>
       </c>
       <c r="AD8" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="AE8" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -3088,25 +3109,25 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F9" t="s">
         <v>31</v>
       </c>
       <c r="H9" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>476</v>
       </c>
       <c r="N9" t="s">
         <v>34</v>
       </c>
       <c r="O9" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="R9" t="s">
         <v>90</v>
@@ -3115,10 +3136,10 @@
         <v>242</v>
       </c>
       <c r="U9" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="X9" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Z9" t="s">
         <v>205</v>
@@ -3127,7 +3148,7 @@
         <v>185</v>
       </c>
       <c r="AE9" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
@@ -3135,34 +3156,34 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I10" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="L10" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="N10" t="s">
         <v>35</v>
       </c>
       <c r="O10" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="R10" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="S10" t="s">
         <v>243</v>
       </c>
       <c r="U10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="Z10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AC10" t="s">
         <v>186</v>
@@ -3173,25 +3194,25 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F11" t="s">
-        <v>251</v>
+        <v>574</v>
       </c>
       <c r="H11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L11" t="s">
-        <v>481</v>
+        <v>37</v>
       </c>
       <c r="N11" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="O11" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="R11" t="s">
         <v>91</v>
@@ -3200,10 +3221,10 @@
         <v>244</v>
       </c>
       <c r="Z11" t="s">
+        <v>253</v>
+      </c>
+      <c r="AC11" t="s">
         <v>254</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>255</v>
       </c>
       <c r="AE11" t="s">
         <v>229</v>
@@ -3214,22 +3235,22 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L12" t="s">
-        <v>385</v>
+        <v>477</v>
       </c>
       <c r="N12" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="O12" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="R12" t="s">
         <v>40</v>
@@ -3249,22 +3270,22 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L13" t="s">
-        <v>17</v>
+        <v>381</v>
       </c>
       <c r="N13" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="R13" t="s">
         <v>92</v>
@@ -3273,13 +3294,13 @@
         <v>250</v>
       </c>
       <c r="Z13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AC13" t="s">
         <v>188</v>
       </c>
       <c r="AE13" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
@@ -3290,16 +3311,16 @@
         <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L14" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="N14" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="R14" t="s">
         <v>93</v>
@@ -3314,27 +3335,27 @@
         <v>189</v>
       </c>
       <c r="AE14" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
       <c r="H15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L15" t="s">
-        <v>482</v>
+        <v>41</v>
       </c>
       <c r="N15" t="s">
         <v>38</v>
       </c>
       <c r="R15" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="S15" t="s">
         <v>247</v>
@@ -3346,27 +3367,27 @@
         <v>190</v>
       </c>
       <c r="AE15" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="F16" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="H16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>478</v>
       </c>
       <c r="N16" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="R16" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="S16" t="s">
         <v>248</v>
@@ -3378,7 +3399,7 @@
         <v>191</v>
       </c>
       <c r="AE16" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
@@ -3386,25 +3407,25 @@
         <v>192</v>
       </c>
       <c r="F17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="H17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N17" t="s">
         <v>39</v>
       </c>
       <c r="Z17" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="AC17" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="AE17" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
@@ -3412,13 +3433,13 @@
         <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H18" t="s">
         <v>87</v>
       </c>
       <c r="L18" t="s">
-        <v>458</v>
+        <v>80</v>
       </c>
       <c r="N18" t="s">
         <v>42</v>
@@ -3427,7 +3448,7 @@
         <v>102</v>
       </c>
       <c r="AE18" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -3441,13 +3462,13 @@
         <v>88</v>
       </c>
       <c r="L19" t="s">
-        <v>81</v>
+        <v>454</v>
       </c>
       <c r="Z19" t="s">
         <v>103</v>
       </c>
       <c r="AE19" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -3458,53 +3479,53 @@
         <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Z20" t="s">
         <v>104</v>
       </c>
       <c r="AE20" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L21" t="s">
-        <v>375</v>
+        <v>82</v>
       </c>
       <c r="Z21" t="s">
         <v>105</v>
       </c>
       <c r="AE21" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F22" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="H22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L22" t="s">
-        <v>465</v>
+        <v>577</v>
       </c>
       <c r="Z22" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="AE22" t="s">
         <v>231</v>
@@ -3512,62 +3533,62 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F23" t="s">
         <v>60</v>
       </c>
       <c r="H23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L23" t="s">
-        <v>43</v>
+        <v>461</v>
       </c>
       <c r="Z23" t="s">
         <v>106</v>
       </c>
       <c r="AE23" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L24" t="s">
-        <v>387</v>
+        <v>43</v>
       </c>
       <c r="Z24" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="AE24" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F25" t="s">
         <v>61</v>
       </c>
       <c r="H25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L25" t="s">
-        <v>519</v>
+        <v>383</v>
       </c>
       <c r="Z25" t="s">
         <v>107</v>
       </c>
       <c r="AE25" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
@@ -3575,13 +3596,13 @@
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H26" t="s">
         <v>74</v>
       </c>
       <c r="L26" t="s">
-        <v>83</v>
+        <v>515</v>
       </c>
       <c r="Z26" t="s">
         <v>108</v>
@@ -3598,10 +3619,10 @@
         <v>221</v>
       </c>
       <c r="H27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L27" t="s">
-        <v>429</v>
+        <v>83</v>
       </c>
       <c r="Z27" t="s">
         <v>109</v>
@@ -3618,10 +3639,10 @@
         <v>222</v>
       </c>
       <c r="H28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L28" t="s">
-        <v>44</v>
+        <v>425</v>
       </c>
       <c r="Z28" t="s">
         <v>110</v>
@@ -3632,27 +3653,30 @@
         <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F30" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H30" t="s">
-        <v>280</v>
+        <v>279</v>
+      </c>
+      <c r="L30" t="s">
+        <v>45</v>
       </c>
       <c r="Z30" t="s">
         <v>111</v>
@@ -3663,7 +3687,7 @@
         <v>223</v>
       </c>
       <c r="F31" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H31" t="s">
         <v>212</v>
@@ -3677,7 +3701,7 @@
         <v>62</v>
       </c>
       <c r="H32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Z32" t="s">
         <v>113</v>
@@ -3688,7 +3712,7 @@
         <v>63</v>
       </c>
       <c r="H33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z33" t="s">
         <v>114</v>
@@ -3699,10 +3723,10 @@
         <v>64</v>
       </c>
       <c r="H34" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="Z34" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="35" spans="6:26" x14ac:dyDescent="0.2">
@@ -3710,7 +3734,7 @@
         <v>65</v>
       </c>
       <c r="H35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z35" t="s">
         <v>115</v>
@@ -3721,7 +3745,7 @@
         <v>66</v>
       </c>
       <c r="H36" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Z36" t="s">
         <v>116</v>
@@ -3732,7 +3756,7 @@
         <v>67</v>
       </c>
       <c r="H37" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Z37" t="s">
         <v>206</v>
@@ -3743,7 +3767,7 @@
         <v>68</v>
       </c>
       <c r="H38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z38" t="s">
         <v>117</v>
@@ -3754,18 +3778,18 @@
         <v>69</v>
       </c>
       <c r="H39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Z39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z40" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="41" spans="6:26" x14ac:dyDescent="0.2">
@@ -3773,7 +3797,7 @@
         <v>76</v>
       </c>
       <c r="Z41" t="s">
-        <v>522</v>
+        <v>580</v>
       </c>
     </row>
     <row r="42" spans="6:26" x14ac:dyDescent="0.2">
@@ -3781,12 +3805,12 @@
         <v>208</v>
       </c>
       <c r="Z42" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H43" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="Z43" t="s">
         <v>118</v>
@@ -3794,7 +3818,7 @@
     </row>
     <row r="44" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Z44" t="s">
         <v>119</v>
@@ -3802,7 +3826,7 @@
     </row>
     <row r="45" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="Z45" t="s">
         <v>120</v>
@@ -3810,7 +3834,7 @@
     </row>
     <row r="46" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="Z46" t="s">
         <v>121</v>
@@ -3818,7 +3842,7 @@
     </row>
     <row r="47" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H47" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Z47" t="s">
         <v>122</v>
@@ -3826,7 +3850,7 @@
     </row>
     <row r="48" spans="6:26" x14ac:dyDescent="0.2">
       <c r="H48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Z48" t="s">
         <v>123</v>
@@ -3837,12 +3861,12 @@
         <v>207</v>
       </c>
       <c r="Z49" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Z50" t="s">
         <v>209</v>
@@ -3850,7 +3874,7 @@
     </row>
     <row r="51" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H51" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Z51" t="s">
         <v>75</v>
@@ -3858,15 +3882,15 @@
     </row>
     <row r="52" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H52" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="Z52" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="53" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="Z53" t="s">
         <v>124</v>
@@ -3874,7 +3898,7 @@
     </row>
     <row r="54" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="Z54" t="s">
         <v>125</v>
@@ -3882,7 +3906,7 @@
     </row>
     <row r="55" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Z55" t="s">
         <v>126</v>
@@ -3890,23 +3914,23 @@
     </row>
     <row r="56" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z56" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="57" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H57" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z57" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="58" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Z58" t="s">
         <v>127</v>
@@ -3914,23 +3938,23 @@
     </row>
     <row r="59" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H59" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="Z59" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="60" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H60" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Z60" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="61" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H61" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z61" t="s">
         <v>128</v>
@@ -3938,7 +3962,7 @@
     </row>
     <row r="62" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Z62" t="s">
         <v>129</v>
@@ -3946,7 +3970,7 @@
     </row>
     <row r="63" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Z63" t="s">
         <v>130</v>
@@ -3954,7 +3978,7 @@
     </row>
     <row r="64" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H64" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Z64" t="s">
         <v>131</v>
@@ -3962,7 +3986,7 @@
     </row>
     <row r="65" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H65" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z65" t="s">
         <v>132</v>
@@ -3970,7 +3994,7 @@
     </row>
     <row r="66" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H66" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="Z66" t="s">
         <v>133</v>
@@ -3978,7 +4002,7 @@
     </row>
     <row r="67" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H67" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="Z67" t="s">
         <v>134</v>
@@ -3986,23 +4010,23 @@
     </row>
     <row r="68" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H68" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Z68" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="69" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H69" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Z69" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="70" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Z70" t="s">
         <v>210</v>
@@ -4010,23 +4034,23 @@
     </row>
     <row r="71" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H71" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="Z71" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="72" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H72" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z72" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="73" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H73" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="Z73" t="s">
         <v>135</v>
@@ -4034,7 +4058,7 @@
     </row>
     <row r="74" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H74" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Z74" t="s">
         <v>136</v>
@@ -4042,7 +4066,7 @@
     </row>
     <row r="75" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H75" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="Z75" t="s">
         <v>137</v>
@@ -4050,7 +4074,7 @@
     </row>
     <row r="76" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H76" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z76" t="s">
         <v>138</v>
@@ -4058,7 +4082,7 @@
     </row>
     <row r="77" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H77" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="Z77" t="s">
         <v>193</v>
@@ -4066,7 +4090,7 @@
     </row>
     <row r="78" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H78" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Z78" t="s">
         <v>194</v>
@@ -4074,23 +4098,23 @@
     </row>
     <row r="79" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H79" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Z79" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="80" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Z80" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="81" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H81" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Z81" t="s">
         <v>139</v>
@@ -4098,7 +4122,7 @@
     </row>
     <row r="82" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H82" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="Z82" t="s">
         <v>140</v>
@@ -4106,7 +4130,7 @@
     </row>
     <row r="83" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H83" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Z83" t="s">
         <v>141</v>
@@ -4114,15 +4138,15 @@
     </row>
     <row r="84" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H84" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z84" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="85" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H85" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Z85" t="s">
         <v>142</v>
@@ -4130,7 +4154,7 @@
     </row>
     <row r="86" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H86" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Z86" t="s">
         <v>143</v>
@@ -4138,7 +4162,7 @@
     </row>
     <row r="87" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H87" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z87" t="s">
         <v>195</v>
@@ -4146,274 +4170,289 @@
     </row>
     <row r="88" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="Z88" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="89" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H89" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z89" t="s">
-        <v>196</v>
+        <v>581</v>
       </c>
     </row>
     <row r="90" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H90" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Z90" t="s">
-        <v>449</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H91" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Z91" t="s">
-        <v>197</v>
+        <v>445</v>
       </c>
     </row>
     <row r="92" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Z92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H93" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Z93" t="s">
-        <v>541</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Z94" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="95" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Z95" t="s">
-        <v>211</v>
+        <v>537</v>
       </c>
     </row>
     <row r="96" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Z96" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Z97" t="s">
-        <v>199</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="8:26" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Z98" t="s">
-        <v>437</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z99" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="100" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z100" t="s">
-        <v>200</v>
+        <v>582</v>
       </c>
     </row>
     <row r="101" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z101" t="s">
-        <v>201</v>
+        <v>583</v>
       </c>
     </row>
     <row r="102" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z102" t="s">
-        <v>202</v>
+        <v>434</v>
       </c>
     </row>
     <row r="103" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z103" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z104" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z105" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z106" t="s">
-        <v>493</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z107" t="s">
-        <v>545</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z108" t="s">
-        <v>517</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z109" t="s">
-        <v>145</v>
+        <v>489</v>
       </c>
     </row>
     <row r="110" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z110" t="s">
-        <v>518</v>
+        <v>540</v>
       </c>
     </row>
     <row r="111" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z111" t="s">
-        <v>378</v>
+        <v>513</v>
       </c>
     </row>
     <row r="112" spans="8:26" x14ac:dyDescent="0.2">
       <c r="Z112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z113" t="s">
-        <v>147</v>
+        <v>514</v>
       </c>
     </row>
     <row r="114" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z114" t="s">
-        <v>148</v>
+        <v>374</v>
       </c>
     </row>
     <row r="115" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z115" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z116" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z117" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="118" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z118" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z119" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z120" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z121" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z122" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z123" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z124" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z125" t="s">
-        <v>439</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z126" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="127" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z127" t="s">
-        <v>539</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z128" t="s">
-        <v>160</v>
+        <v>435</v>
       </c>
     </row>
     <row r="129" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z129" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="130" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z130" t="s">
-        <v>162</v>
+        <v>534</v>
       </c>
     </row>
     <row r="131" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z131" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z132" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z133" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="134" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z134" t="s">
-        <v>165</v>
+        <v>46</v>
       </c>
     </row>
     <row r="135" spans="26:26" x14ac:dyDescent="0.2">
       <c r="Z135" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="136" spans="26:26" x14ac:dyDescent="0.2">
+      <c r="Z136" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="137" spans="26:26" x14ac:dyDescent="0.2">
+      <c r="Z137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="138" spans="26:26" x14ac:dyDescent="0.2">
+      <c r="Z138" t="s">
         <v>166</v>
       </c>
     </row>
@@ -4428,7 +4467,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4436,9 +4475,11 @@
     <col min="1" max="1" width="20.5" style="28" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="50" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9.6640625" style="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.1640625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="49.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="20.1640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.1640625" style="10" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="49.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="20.1640625" style="10" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="41" style="23" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="1.6640625" style="11" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12" style="16" customWidth="1" collapsed="1"/>
@@ -4462,10 +4503,10 @@
         <v>20</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>19</v>
@@ -4481,7 +4522,7 @@
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -4491,7 +4532,7 @@
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
       <c r="I2" s="26" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="3"/>
@@ -4564,27 +4605,29 @@
     </row>
     <row r="5" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>375</v>
+        <v>577</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="H5" s="7"/>
+        <v>544</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>584</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="22"/>
       <c r="K5" s="3"/>
@@ -4603,10 +4646,10 @@
         <v>61</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -4621,19 +4664,19 @@
     <row r="7" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="29" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -4652,13 +4695,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -4680,10 +4723,10 @@
         <v>37</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -4698,7 +4741,7 @@
     <row r="10" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="29" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>50</v>
@@ -4707,10 +4750,10 @@
         <v>40</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -4725,24 +4768,26 @@
     <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27"/>
       <c r="B11" s="5" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>375</v>
+        <v>577</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="H11" s="7"/>
+        <v>544</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>584</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="22"/>
       <c r="K11" s="3"/>
@@ -4751,7 +4796,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="5"/>
       <c r="C12" s="13" t="s">
@@ -4761,14 +4806,14 @@
         <v>68</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="22" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="15"/>
@@ -4778,10 +4823,10 @@
     </row>
     <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>13</v>
@@ -4790,10 +4835,10 @@
         <v>61</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -4812,18 +4857,20 @@
         <v>14</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>375</v>
+        <v>577</v>
       </c>
       <c r="E14" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>568</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>569</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>573</v>
-      </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>584</v>
+      </c>
       <c r="I14" s="7"/>
       <c r="J14" s="22"/>
       <c r="K14" s="3"/>
@@ -4842,10 +4889,10 @@
         <v>61</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -4860,19 +4907,19 @@
     <row r="16" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="29" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -4891,13 +4938,13 @@
         <v>13</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -4919,10 +4966,10 @@
         <v>37</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -4937,7 +4984,7 @@
     <row r="19" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="29" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>50</v>
@@ -4946,10 +4993,10 @@
         <v>40</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -4964,24 +5011,26 @@
     <row r="20" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="5" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>375</v>
+        <v>577</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>573</v>
-      </c>
-      <c r="H20" s="7"/>
+        <v>568</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>584</v>
+      </c>
       <c r="I20" s="7"/>
       <c r="J20" s="22"/>
       <c r="K20" s="3"/>
@@ -5000,14 +5049,14 @@
         <v>68</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="22" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="15"/>

</xml_diff>